<commit_message>
slides and documents from S98 mtg 21/11/25
</commit_message>
<xml_diff>
--- a/documents/2.0.0/S-98 Comments June 2025.xlsx
+++ b/documents/2.0.0/S-98 Comments June 2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\kusal\98-interoperability\documents\2.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D698E775-9C58-4F18-8F5B-169210FBDDAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568102FC-5B8D-4510-9268-92F13F757F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-66048" yWindow="1236" windowWidth="40296" windowHeight="20724" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-102744" yWindow="744" windowWidth="33084" windowHeight="22392" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original_Comments 11032025" sheetId="1" r:id="rId1"/>
@@ -9655,7 +9655,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="113.15">
+    <row r="60" spans="1:9" ht="102.9">
       <c r="A60" s="135"/>
       <c r="B60" s="140"/>
       <c r="C60" s="147" t="s">
@@ -21222,8 +21222,8 @@
   <dimension ref="A1:AB1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I133" sqref="I133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.69140625" defaultRowHeight="12.45"/>
@@ -21411,7 +21411,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="133.75">
+    <row r="5" spans="1:28" ht="133.75" hidden="1">
       <c r="A5" s="27"/>
       <c r="B5" s="4" t="str">
         <f t="shared" si="0"/>
@@ -21752,7 +21752,7 @@
       <c r="M13" s="13"/>
       <c r="N13" s="14"/>
     </row>
-    <row r="14" spans="1:28" ht="102.9">
+    <row r="14" spans="1:28" ht="102.9" hidden="1">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="str">
         <f t="shared" si="0"/>
@@ -21793,7 +21793,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="92.6">
+    <row r="15" spans="1:28" ht="92.6" hidden="1">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="str">
         <f t="shared" si="0"/>
@@ -21836,7 +21836,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="113.15">
+    <row r="16" spans="1:28" ht="102.9" hidden="1">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="str">
         <f t="shared" si="0"/>
@@ -22384,7 +22384,7 @@
       <c r="M29" s="13"/>
       <c r="N29" s="14"/>
     </row>
-    <row r="30" spans="1:14" ht="20.6" hidden="1">
+    <row r="30" spans="1:14" ht="20.6">
       <c r="A30" s="4"/>
       <c r="B30" s="4" t="str">
         <f t="shared" si="0"/>
@@ -22655,7 +22655,7 @@
       <c r="M36" s="13"/>
       <c r="N36" s="14"/>
     </row>
-    <row r="37" spans="1:14" ht="185.15" hidden="1">
+    <row r="37" spans="1:14" ht="174.9" hidden="1">
       <c r="A37" s="4"/>
       <c r="B37" s="4" t="str">
         <f t="shared" si="0"/>
@@ -23078,7 +23078,7 @@
         <v>1418</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="216">
+    <row r="48" spans="1:14" ht="216" hidden="1">
       <c r="A48" s="22"/>
       <c r="B48" s="4" t="str">
         <f t="shared" si="0"/>
@@ -23154,7 +23154,7 @@
       <c r="M49" s="13"/>
       <c r="N49" s="14"/>
     </row>
-    <row r="50" spans="1:14" ht="30.9">
+    <row r="50" spans="1:14" ht="30.9" hidden="1">
       <c r="A50" s="4"/>
       <c r="B50" s="4" t="str">
         <f t="shared" si="0"/>
@@ -23593,7 +23593,7 @@
         <v>1425</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="30.9">
+    <row r="61" spans="1:14" ht="30.9" hidden="1">
       <c r="A61" s="27" t="s">
         <v>674</v>
       </c>
@@ -23714,7 +23714,7 @@
       <c r="M63" s="13"/>
       <c r="N63" s="14"/>
     </row>
-    <row r="64" spans="1:14" ht="41.15">
+    <row r="64" spans="1:14" ht="41.15" hidden="1">
       <c r="A64" s="4"/>
       <c r="B64" s="4" t="str">
         <f t="shared" si="0"/>
@@ -23755,7 +23755,7 @@
       </c>
       <c r="N64" s="14"/>
     </row>
-    <row r="65" spans="1:14" ht="41.15">
+    <row r="65" spans="1:14" ht="41.15" hidden="1">
       <c r="A65" s="22"/>
       <c r="B65" s="4" t="str">
         <f t="shared" si="0"/>
@@ -23874,7 +23874,7 @@
       <c r="M67" s="13"/>
       <c r="N67" s="14"/>
     </row>
-    <row r="68" spans="1:14" ht="133.75">
+    <row r="68" spans="1:14" ht="133.75" hidden="1">
       <c r="A68" s="4"/>
       <c r="B68" s="4" t="str">
         <f t="shared" si="1"/>
@@ -23913,7 +23913,7 @@
       </c>
       <c r="N68" s="14"/>
     </row>
-    <row r="69" spans="1:14" ht="30.9">
+    <row r="69" spans="1:14" ht="30.9" hidden="1">
       <c r="A69" s="4"/>
       <c r="B69" s="4" t="str">
         <f t="shared" si="1"/>
@@ -23991,7 +23991,7 @@
       </c>
       <c r="N70" s="14"/>
     </row>
-    <row r="71" spans="1:14" ht="185.15">
+    <row r="71" spans="1:14" ht="185.15" hidden="1">
       <c r="A71" s="4"/>
       <c r="B71" s="4" t="str">
         <f t="shared" si="1"/>
@@ -24073,7 +24073,7 @@
         <v>1464</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="32.15">
+    <row r="73" spans="1:14" ht="32.15" hidden="1">
       <c r="A73" s="4"/>
       <c r="B73" s="4" t="str">
         <f t="shared" si="1"/>
@@ -24305,7 +24305,7 @@
       <c r="M78" s="13"/>
       <c r="N78" s="14"/>
     </row>
-    <row r="79" spans="1:14" ht="298.3">
+    <row r="79" spans="1:14" ht="298.3" hidden="1">
       <c r="A79" s="22"/>
       <c r="B79" s="4" t="str">
         <f t="shared" si="1"/>
@@ -24422,7 +24422,7 @@
       <c r="M81" s="13"/>
       <c r="N81" s="14"/>
     </row>
-    <row r="82" spans="1:14" ht="318.89999999999998">
+    <row r="82" spans="1:14" ht="318.89999999999998" hidden="1">
       <c r="A82" s="22"/>
       <c r="B82" s="4" t="str">
         <f t="shared" si="1"/>
@@ -24765,7 +24765,7 @@
       <c r="M90" s="13"/>
       <c r="N90" s="14"/>
     </row>
-    <row r="91" spans="1:14" ht="20.6" hidden="1">
+    <row r="91" spans="1:14" ht="20.6">
       <c r="A91" s="4"/>
       <c r="B91" s="4" t="str">
         <f t="shared" si="1"/>
@@ -25038,7 +25038,7 @@
       </c>
       <c r="N97" s="14"/>
     </row>
-    <row r="98" spans="1:14" ht="61.75">
+    <row r="98" spans="1:14" ht="61.75" hidden="1">
       <c r="A98" s="22"/>
       <c r="B98" s="4" t="str">
         <f t="shared" si="1"/>
@@ -25153,7 +25153,7 @@
       </c>
       <c r="N100" s="14"/>
     </row>
-    <row r="101" spans="1:14" ht="41.15">
+    <row r="101" spans="1:14" ht="41.15" hidden="1">
       <c r="A101" s="4"/>
       <c r="B101" s="4" t="str">
         <f t="shared" si="1"/>
@@ -25229,7 +25229,7 @@
       </c>
       <c r="N102" s="14"/>
     </row>
-    <row r="103" spans="1:14" ht="51.45">
+    <row r="103" spans="1:14" ht="51.45" hidden="1">
       <c r="A103" s="4"/>
       <c r="B103" s="4" t="str">
         <f t="shared" si="1"/>
@@ -25599,7 +25599,7 @@
       <c r="M112" s="13"/>
       <c r="N112" s="14"/>
     </row>
-    <row r="113" spans="1:14" ht="61.75">
+    <row r="113" spans="1:14" ht="61.75" hidden="1">
       <c r="A113" s="22"/>
       <c r="B113" s="4" t="str">
         <f t="shared" si="1"/>
@@ -25858,7 +25858,7 @@
       <c r="M119" s="13"/>
       <c r="N119" s="14"/>
     </row>
-    <row r="120" spans="1:14" ht="37.299999999999997">
+    <row r="120" spans="1:14" ht="37.299999999999997" hidden="1">
       <c r="A120" s="4"/>
       <c r="B120" s="4" t="str">
         <f t="shared" si="1"/>
@@ -26088,7 +26088,7 @@
       <c r="M125" s="13"/>
       <c r="N125" s="14"/>
     </row>
-    <row r="126" spans="1:14" ht="82.3">
+    <row r="126" spans="1:14" ht="82.3" hidden="1">
       <c r="A126" s="4"/>
       <c r="B126" s="4" t="str">
         <f t="shared" si="1"/>
@@ -26129,7 +26129,7 @@
         <v>1531</v>
       </c>
     </row>
-    <row r="127" spans="1:14" ht="41.15">
+    <row r="127" spans="1:14" ht="41.15" hidden="1">
       <c r="A127" s="4"/>
       <c r="B127" s="4" t="str">
         <f t="shared" si="1"/>
@@ -26207,7 +26207,7 @@
       <c r="M128" s="13"/>
       <c r="N128" s="14"/>
     </row>
-    <row r="129" spans="1:14" ht="30.9">
+    <row r="129" spans="1:14" ht="30.9" hidden="1">
       <c r="A129" s="4"/>
       <c r="B129" s="4" t="str">
         <f t="shared" si="1"/>
@@ -26289,7 +26289,7 @@
       </c>
       <c r="N130" s="14"/>
     </row>
-    <row r="131" spans="1:14" ht="51.45" hidden="1">
+    <row r="131" spans="1:14" ht="51.45">
       <c r="A131" s="4"/>
       <c r="B131" s="4" t="str">
         <f t="shared" ref="B131:B194" si="2">IF(ISNUMBER(SEARCH("DONE",K131)),"DONE","")</f>
@@ -26328,7 +26328,7 @@
       <c r="M131" s="13"/>
       <c r="N131" s="14"/>
     </row>
-    <row r="132" spans="1:14" ht="51.45" hidden="1">
+    <row r="132" spans="1:14" ht="51.45">
       <c r="A132" s="4"/>
       <c r="B132" s="4" t="str">
         <f t="shared" si="2"/>
@@ -26367,7 +26367,7 @@
       <c r="M132" s="13"/>
       <c r="N132" s="14"/>
     </row>
-    <row r="133" spans="1:14" ht="30.9" hidden="1">
+    <row r="133" spans="1:14" ht="30.9">
       <c r="A133" s="4"/>
       <c r="B133" s="4" t="str">
         <f t="shared" si="2"/>
@@ -26408,7 +26408,7 @@
       </c>
       <c r="N133" s="14"/>
     </row>
-    <row r="134" spans="1:14" ht="20.6" hidden="1">
+    <row r="134" spans="1:14" ht="20.6">
       <c r="A134" s="4"/>
       <c r="B134" s="4" t="str">
         <f t="shared" si="2"/>
@@ -26521,7 +26521,7 @@
       <c r="M136" s="13"/>
       <c r="N136" s="14"/>
     </row>
-    <row r="137" spans="1:14" hidden="1">
+    <row r="137" spans="1:14">
       <c r="A137" s="4"/>
       <c r="B137" s="4" t="str">
         <f t="shared" si="2"/>
@@ -26817,7 +26817,7 @@
         <v>1572</v>
       </c>
     </row>
-    <row r="145" spans="1:14" ht="41.15">
+    <row r="145" spans="1:14" ht="41.15" hidden="1">
       <c r="A145" s="22"/>
       <c r="B145" s="4" t="str">
         <f t="shared" si="2"/>
@@ -26899,7 +26899,7 @@
         <v>1418</v>
       </c>
     </row>
-    <row r="147" spans="1:14" ht="41.15" hidden="1">
+    <row r="147" spans="1:14" ht="41.15">
       <c r="A147" s="4"/>
       <c r="B147" s="4" t="str">
         <f t="shared" si="2"/>
@@ -27057,7 +27057,7 @@
       </c>
       <c r="N150" s="14"/>
     </row>
-    <row r="151" spans="1:14" ht="51.45">
+    <row r="151" spans="1:14" ht="51.45" hidden="1">
       <c r="A151" s="22"/>
       <c r="B151" s="4" t="str">
         <f t="shared" si="2"/>
@@ -27427,7 +27427,7 @@
       <c r="M160" s="13"/>
       <c r="N160" s="14"/>
     </row>
-    <row r="161" spans="1:14" ht="20.6" hidden="1">
+    <row r="161" spans="1:14" ht="20.6">
       <c r="A161" s="4"/>
       <c r="B161" s="4" t="str">
         <f t="shared" si="2"/>
@@ -27505,7 +27505,7 @@
       <c r="M162" s="13"/>
       <c r="N162" s="14"/>
     </row>
-    <row r="163" spans="1:14" ht="41.15" hidden="1">
+    <row r="163" spans="1:14" ht="41.15">
       <c r="A163" s="4"/>
       <c r="B163" s="4" t="str">
         <f t="shared" si="2"/>
@@ -27548,7 +27548,7 @@
         <v>1595</v>
       </c>
     </row>
-    <row r="164" spans="1:14" hidden="1">
+    <row r="164" spans="1:14">
       <c r="A164" s="4"/>
       <c r="B164" s="4" t="str">
         <f t="shared" si="2"/>
@@ -27667,7 +27667,7 @@
       <c r="M166" s="13"/>
       <c r="N166" s="14"/>
     </row>
-    <row r="167" spans="1:14" ht="20.6">
+    <row r="167" spans="1:14" ht="20.6" hidden="1">
       <c r="A167" s="4"/>
       <c r="B167" s="4" t="str">
         <f t="shared" si="2"/>
@@ -27885,7 +27885,7 @@
       <c r="M172" s="13"/>
       <c r="N172" s="14"/>
     </row>
-    <row r="173" spans="1:14" ht="51.45">
+    <row r="173" spans="1:14" ht="51.45" hidden="1">
       <c r="A173" s="4"/>
       <c r="B173" s="4" t="str">
         <f t="shared" si="2"/>
@@ -28107,7 +28107,7 @@
       <c r="M178" s="13"/>
       <c r="N178" s="14"/>
     </row>
-    <row r="179" spans="1:14" ht="30.9">
+    <row r="179" spans="1:14" ht="30.9" hidden="1">
       <c r="A179" s="22"/>
       <c r="B179" s="4" t="str">
         <f t="shared" si="2"/>
@@ -28181,7 +28181,7 @@
       <c r="M180" s="13"/>
       <c r="N180" s="14"/>
     </row>
-    <row r="181" spans="1:14" ht="72" hidden="1">
+    <row r="181" spans="1:14" ht="72">
       <c r="A181" s="4"/>
       <c r="B181" s="4" t="str">
         <f t="shared" si="2"/>
@@ -28329,7 +28329,7 @@
         <v>1595</v>
       </c>
     </row>
-    <row r="185" spans="1:14" ht="51.45" hidden="1">
+    <row r="185" spans="1:14" ht="51.45">
       <c r="A185" s="4"/>
       <c r="B185" s="4" t="str">
         <f t="shared" si="2"/>
@@ -28588,7 +28588,7 @@
       <c r="M191" s="13"/>
       <c r="N191" s="14"/>
     </row>
-    <row r="192" spans="1:14" ht="144">
+    <row r="192" spans="1:14" ht="144" hidden="1">
       <c r="A192" s="4"/>
       <c r="B192" s="4" t="str">
         <f t="shared" si="2"/>
@@ -28627,7 +28627,7 @@
         <v>1595</v>
       </c>
     </row>
-    <row r="193" spans="1:14">
+    <row r="193" spans="1:14" hidden="1">
       <c r="A193" s="4"/>
       <c r="B193" s="4" t="str">
         <f t="shared" si="2"/>
@@ -28701,7 +28701,7 @@
       <c r="M194" s="13"/>
       <c r="N194" s="14"/>
     </row>
-    <row r="195" spans="1:14" ht="20.6">
+    <row r="195" spans="1:14" ht="20.6" hidden="1">
       <c r="A195" s="22"/>
       <c r="B195" s="4" t="str">
         <f t="shared" ref="B195:B258" si="3">IF(ISNUMBER(SEARCH("DONE",K195)),"DONE","")</f>
@@ -28738,7 +28738,7 @@
       </c>
       <c r="N195" s="14"/>
     </row>
-    <row r="196" spans="1:14" ht="30.9">
+    <row r="196" spans="1:14" ht="30.9" hidden="1">
       <c r="A196" s="4"/>
       <c r="B196" s="4" t="str">
         <f t="shared" si="3"/>
@@ -28845,7 +28845,7 @@
       <c r="M198" s="13"/>
       <c r="N198" s="14"/>
     </row>
-    <row r="199" spans="1:14" ht="41.15">
+    <row r="199" spans="1:14" ht="41.15" hidden="1">
       <c r="A199" s="4"/>
       <c r="B199" s="4" t="str">
         <f t="shared" si="3"/>
@@ -28882,7 +28882,7 @@
       <c r="M199" s="13"/>
       <c r="N199" s="14"/>
     </row>
-    <row r="200" spans="1:14" ht="30.9" hidden="1">
+    <row r="200" spans="1:14" ht="30.9">
       <c r="A200" s="4"/>
       <c r="B200" s="4" t="str">
         <f t="shared" si="3"/>
@@ -28995,7 +28995,7 @@
       <c r="M202" s="13"/>
       <c r="N202" s="14"/>
     </row>
-    <row r="203" spans="1:14" ht="20.6">
+    <row r="203" spans="1:14" ht="20.6" hidden="1">
       <c r="A203" s="4"/>
       <c r="B203" s="4" t="str">
         <f t="shared" si="3"/>
@@ -29032,7 +29032,7 @@
       <c r="M203" s="13"/>
       <c r="N203" s="14"/>
     </row>
-    <row r="204" spans="1:14" ht="21.45">
+    <row r="204" spans="1:14" ht="21.45" hidden="1">
       <c r="A204" s="4"/>
       <c r="B204" s="4" t="str">
         <f t="shared" si="3"/>
@@ -29149,7 +29149,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="207" spans="1:14" ht="41.15">
+    <row r="207" spans="1:14" ht="41.15" hidden="1">
       <c r="A207" s="27"/>
       <c r="B207" s="4" t="str">
         <f t="shared" si="3"/>
@@ -29379,7 +29379,7 @@
       <c r="M212" s="13"/>
       <c r="N212" s="14"/>
     </row>
-    <row r="213" spans="1:14" ht="21.45" hidden="1">
+    <row r="213" spans="1:14" ht="21.45">
       <c r="A213" s="4"/>
       <c r="B213" s="4" t="str">
         <f t="shared" si="3"/>
@@ -29422,7 +29422,7 @@
         <v>1418</v>
       </c>
     </row>
-    <row r="214" spans="1:14" ht="41.15">
+    <row r="214" spans="1:14" ht="41.15" hidden="1">
       <c r="A214" s="4"/>
       <c r="B214" s="4" t="str">
         <f t="shared" si="3"/>
@@ -29461,7 +29461,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="215" spans="1:14" ht="30.9">
+    <row r="215" spans="1:14" ht="30.9" hidden="1">
       <c r="A215" s="4"/>
       <c r="B215" s="4" t="str">
         <f t="shared" si="3"/>
@@ -29695,7 +29695,7 @@
       </c>
       <c r="N220" s="14"/>
     </row>
-    <row r="221" spans="1:14" ht="21.45" hidden="1">
+    <row r="221" spans="1:14" ht="21.45">
       <c r="A221" s="4"/>
       <c r="B221" s="4" t="str">
         <f t="shared" si="3"/>
@@ -29736,7 +29736,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="222" spans="1:14" ht="154.30000000000001">
+    <row r="222" spans="1:14" ht="154.30000000000001" hidden="1">
       <c r="A222" s="4"/>
       <c r="B222" s="4" t="str">
         <f t="shared" si="3"/>
@@ -29777,7 +29777,7 @@
         <v>1418</v>
       </c>
     </row>
-    <row r="223" spans="1:14" ht="51.45" hidden="1">
+    <row r="223" spans="1:14" ht="51.45">
       <c r="A223" s="4"/>
       <c r="B223" s="4" t="str">
         <f t="shared" si="3"/>
@@ -30015,7 +30015,7 @@
       <c r="M228" s="13"/>
       <c r="N228" s="14"/>
     </row>
-    <row r="229" spans="1:14" ht="41.15">
+    <row r="229" spans="1:14" ht="41.15" hidden="1">
       <c r="A229" s="4"/>
       <c r="B229" s="4" t="str">
         <f t="shared" si="3"/>
@@ -30054,7 +30054,7 @@
         <v>1418</v>
       </c>
     </row>
-    <row r="230" spans="1:14" ht="113.15">
+    <row r="230" spans="1:14" ht="113.15" hidden="1">
       <c r="A230" s="4"/>
       <c r="B230" s="4" t="str">
         <f t="shared" si="3"/>
@@ -30173,7 +30173,7 @@
         <v>1418</v>
       </c>
     </row>
-    <row r="233" spans="1:14" ht="20.6" hidden="1">
+    <row r="233" spans="1:14" ht="20.6">
       <c r="A233" s="4"/>
       <c r="B233" s="4" t="str">
         <f t="shared" si="3"/>
@@ -30586,7 +30586,7 @@
       <c r="M243" s="13"/>
       <c r="N243" s="14"/>
     </row>
-    <row r="244" spans="1:14" ht="30.9">
+    <row r="244" spans="1:14" ht="30.9" hidden="1">
       <c r="A244" s="27"/>
       <c r="B244" s="4" t="str">
         <f t="shared" si="3"/>
@@ -31456,7 +31456,7 @@
       </c>
       <c r="N265" s="14"/>
     </row>
-    <row r="266" spans="1:14" hidden="1">
+    <row r="266" spans="1:14">
       <c r="A266" s="4"/>
       <c r="B266" s="4" t="str">
         <f t="shared" si="4"/>
@@ -31657,7 +31657,7 @@
       </c>
       <c r="N270" s="14"/>
     </row>
-    <row r="271" spans="1:14" ht="164.6">
+    <row r="271" spans="1:14" ht="164.6" hidden="1">
       <c r="A271" s="4"/>
       <c r="B271" s="4" t="str">
         <f t="shared" si="4"/>
@@ -31928,7 +31928,7 @@
       </c>
       <c r="N277" s="14"/>
     </row>
-    <row r="278" spans="1:14" ht="92.6">
+    <row r="278" spans="1:14" ht="92.6" hidden="1">
       <c r="A278" s="4"/>
       <c r="B278" s="4" t="str">
         <f t="shared" si="4"/>
@@ -32201,7 +32201,7 @@
       <c r="M284" s="13"/>
       <c r="N284" s="14"/>
     </row>
-    <row r="285" spans="1:14" ht="174.9">
+    <row r="285" spans="1:14" ht="174.9" hidden="1">
       <c r="A285" s="22"/>
       <c r="B285" s="4" t="str">
         <f t="shared" si="4"/>
@@ -32536,7 +32536,7 @@
       <c r="M293" s="13"/>
       <c r="N293" s="14"/>
     </row>
-    <row r="294" spans="1:14" ht="123.45">
+    <row r="294" spans="1:14" ht="123.45" hidden="1">
       <c r="A294" s="22"/>
       <c r="B294" s="4" t="str">
         <f t="shared" si="4"/>
@@ -32577,7 +32577,7 @@
         <v>1841</v>
       </c>
     </row>
-    <row r="295" spans="1:14" ht="30.9">
+    <row r="295" spans="1:14" ht="30.9" hidden="1">
       <c r="A295" s="22"/>
       <c r="B295" s="4" t="str">
         <f t="shared" si="4"/>
@@ -32768,7 +32768,7 @@
       </c>
       <c r="N299" s="14"/>
     </row>
-    <row r="300" spans="1:14" ht="30.9" hidden="1">
+    <row r="300" spans="1:14" ht="30.9">
       <c r="A300" s="4"/>
       <c r="B300" s="4" t="str">
         <f t="shared" si="4"/>
@@ -32992,7 +32992,7 @@
       <c r="M305" s="13"/>
       <c r="N305" s="14"/>
     </row>
-    <row r="306" spans="1:14" ht="14.15">
+    <row r="306" spans="1:14" ht="14.15" hidden="1">
       <c r="A306" s="22"/>
       <c r="B306" s="4" t="str">
         <f t="shared" si="4"/>
@@ -33066,7 +33066,7 @@
       <c r="M307" s="13"/>
       <c r="N307" s="14"/>
     </row>
-    <row r="308" spans="1:14" hidden="1">
+    <row r="308" spans="1:14">
       <c r="A308" s="4"/>
       <c r="B308" s="4" t="str">
         <f t="shared" si="4"/>
@@ -33255,7 +33255,7 @@
       <c r="M312" s="13"/>
       <c r="N312" s="14"/>
     </row>
-    <row r="313" spans="1:14" ht="20.6" hidden="1">
+    <row r="313" spans="1:14" ht="20.6">
       <c r="A313" s="75"/>
       <c r="B313" s="4" t="str">
         <f t="shared" si="4"/>
@@ -33296,7 +33296,7 @@
       </c>
       <c r="N313" s="14"/>
     </row>
-    <row r="314" spans="1:14" ht="92.6" hidden="1">
+    <row r="314" spans="1:14" ht="92.6">
       <c r="A314" s="4"/>
       <c r="B314" s="4" t="str">
         <f t="shared" si="4"/>
@@ -33337,7 +33337,7 @@
       </c>
       <c r="N314" s="14"/>
     </row>
-    <row r="315" spans="1:14" hidden="1">
+    <row r="315" spans="1:14">
       <c r="A315" s="4"/>
       <c r="B315" s="4" t="str">
         <f t="shared" si="4"/>
@@ -33374,7 +33374,7 @@
       <c r="M315" s="13"/>
       <c r="N315" s="14"/>
     </row>
-    <row r="316" spans="1:14" hidden="1">
+    <row r="316" spans="1:14">
       <c r="A316" s="4"/>
       <c r="B316" s="4" t="str">
         <f t="shared" si="4"/>
@@ -33411,7 +33411,7 @@
       <c r="M316" s="13"/>
       <c r="N316" s="14"/>
     </row>
-    <row r="317" spans="1:14" ht="41.15" hidden="1">
+    <row r="317" spans="1:14" ht="41.15">
       <c r="A317" s="4"/>
       <c r="B317" s="4" t="str">
         <f t="shared" si="4"/>
@@ -33446,7 +33446,7 @@
       <c r="M317" s="13"/>
       <c r="N317" s="14"/>
     </row>
-    <row r="318" spans="1:14" ht="20.6" hidden="1">
+    <row r="318" spans="1:14" ht="20.6">
       <c r="A318" s="4"/>
       <c r="B318" s="4" t="str">
         <f t="shared" si="4"/>
@@ -33596,7 +33596,7 @@
       <c r="M321" s="13"/>
       <c r="N321" s="14"/>
     </row>
-    <row r="322" spans="1:14" ht="61.75">
+    <row r="322" spans="1:14" ht="61.75" hidden="1">
       <c r="A322" s="4"/>
       <c r="B322" s="4" t="str">
         <f t="shared" si="4"/>
@@ -33711,7 +33711,7 @@
       <c r="M324" s="13"/>
       <c r="N324" s="14"/>
     </row>
-    <row r="325" spans="1:14" ht="20.6">
+    <row r="325" spans="1:14" ht="20.6" hidden="1">
       <c r="A325" s="4"/>
       <c r="B325" s="4" t="str">
         <f t="shared" si="5"/>
@@ -33750,7 +33750,7 @@
       </c>
       <c r="N325" s="14"/>
     </row>
-    <row r="326" spans="1:14">
+    <row r="326" spans="1:14" hidden="1">
       <c r="A326" s="4"/>
       <c r="B326" s="4" t="str">
         <f t="shared" si="5"/>
@@ -35268,7 +35268,7 @@
         <v>1418</v>
       </c>
     </row>
-    <row r="366" spans="1:14" ht="82.3">
+    <row r="366" spans="1:14" ht="82.3" hidden="1">
       <c r="A366" s="22"/>
       <c r="B366" s="4" t="str">
         <f t="shared" si="5"/>
@@ -35309,7 +35309,7 @@
         <v>1418</v>
       </c>
     </row>
-    <row r="367" spans="1:14" ht="30.9">
+    <row r="367" spans="1:14" ht="30.9" hidden="1">
       <c r="A367" s="22"/>
       <c r="B367" s="4" t="str">
         <f t="shared" si="5"/>
@@ -35982,7 +35982,7 @@
       </c>
       <c r="N383" s="14"/>
     </row>
-    <row r="384" spans="1:28" ht="30.9" hidden="1">
+    <row r="384" spans="1:28" ht="30.9">
       <c r="A384" s="4"/>
       <c r="B384" s="4" t="str">
         <f t="shared" si="5"/>
@@ -36278,7 +36278,7 @@
       <c r="M391" s="13"/>
       <c r="N391" s="14"/>
     </row>
-    <row r="392" spans="1:14" ht="92.6">
+    <row r="392" spans="1:14" ht="92.6" hidden="1">
       <c r="A392" s="4"/>
       <c r="B392" s="4" t="str">
         <f t="shared" si="6"/>
@@ -36317,7 +36317,7 @@
       </c>
       <c r="N392" s="14"/>
     </row>
-    <row r="393" spans="1:14" ht="41.15" hidden="1">
+    <row r="393" spans="1:14" ht="41.15">
       <c r="A393" s="4"/>
       <c r="B393" s="4" t="str">
         <f t="shared" si="6"/>
@@ -36537,7 +36537,7 @@
       <c r="M398" s="13"/>
       <c r="N398" s="14"/>
     </row>
-    <row r="399" spans="1:14" ht="82.3">
+    <row r="399" spans="1:14" ht="82.3" hidden="1">
       <c r="A399" s="4"/>
       <c r="B399" s="4" t="str">
         <f t="shared" si="6"/>
@@ -36574,7 +36574,7 @@
       </c>
       <c r="N399" s="14"/>
     </row>
-    <row r="400" spans="1:14" ht="51.45" hidden="1">
+    <row r="400" spans="1:14" ht="51.45">
       <c r="A400" s="4"/>
       <c r="B400" s="4" t="str">
         <f t="shared" si="6"/>
@@ -36796,7 +36796,7 @@
       <c r="M405" s="13"/>
       <c r="N405" s="14"/>
     </row>
-    <row r="406" spans="1:14" ht="30.9">
+    <row r="406" spans="1:14" ht="30.9" hidden="1">
       <c r="A406" s="4"/>
       <c r="B406" s="4" t="str">
         <f t="shared" si="6"/>
@@ -36835,7 +36835,7 @@
       </c>
       <c r="N406" s="14"/>
     </row>
-    <row r="407" spans="1:14" ht="41.15" hidden="1">
+    <row r="407" spans="1:14" ht="41.15">
       <c r="A407" s="4"/>
       <c r="B407" s="4" t="str">
         <f t="shared" si="6"/>
@@ -37423,7 +37423,7 @@
       </c>
       <c r="N422" s="14"/>
     </row>
-    <row r="423" spans="1:14" ht="61.75">
+    <row r="423" spans="1:14" ht="61.75" hidden="1">
       <c r="A423" s="4"/>
       <c r="B423" s="4" t="str">
         <f t="shared" si="6"/>
@@ -37462,7 +37462,7 @@
       </c>
       <c r="N423" s="14"/>
     </row>
-    <row r="424" spans="1:14" ht="72">
+    <row r="424" spans="1:14" ht="72" hidden="1">
       <c r="A424" s="4"/>
       <c r="B424" s="4" t="str">
         <f t="shared" si="6"/>
@@ -37501,7 +37501,7 @@
       </c>
       <c r="N424" s="14"/>
     </row>
-    <row r="425" spans="1:14" ht="61.75">
+    <row r="425" spans="1:14" ht="61.75" hidden="1">
       <c r="A425" s="4"/>
       <c r="B425" s="4" t="str">
         <f t="shared" si="6"/>
@@ -48060,7 +48060,37 @@
     </filterColumn>
     <filterColumn colId="3">
       <filters>
-        <filter val="SM"/>
+        <filter val="DE 11"/>
+        <filter val="DE 12"/>
+        <filter val="DE 13"/>
+        <filter val="DE 16"/>
+        <filter val="DE 20"/>
+        <filter val="DE 24"/>
+        <filter val="DE 37"/>
+        <filter val="DE 38"/>
+        <filter val="DE 39"/>
+        <filter val="DE 40"/>
+        <filter val="DE 41"/>
+        <filter val="DE 42"/>
+        <filter val="DE 47"/>
+        <filter val="DE 48"/>
+        <filter val="DE 51"/>
+        <filter val="DE 52"/>
+        <filter val="DE 54"/>
+        <filter val="DE 58"/>
+        <filter val="DE 59"/>
+        <filter val="DE 60"/>
+        <filter val="DE 61"/>
+        <filter val="DE 62"/>
+        <filter val="DE 63"/>
+        <filter val="DE 67"/>
+        <filter val="DE 68"/>
+        <filter val="DE 69"/>
+        <filter val="DE 70"/>
+        <filter val="DE3"/>
+        <filter val="DE5"/>
+        <filter val="DE6"/>
+        <filter val="DE9"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>